<commit_message>
Added units to several figures.
</commit_message>
<xml_diff>
--- a/Database_BMJ_Open_25Jul2014.xlsx
+++ b/Database_BMJ_Open_25Jul2014.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austin/Desktop/ProCal_Analysis/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austin/Google Drive/Documents/PostPostDoc/pneumococcal_colonization_analysis_redo/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="80" yWindow="460" windowWidth="29660" windowHeight="20540"/>
+    <workbookView xWindow="14000" yWindow="460" windowWidth="29660" windowHeight="20540"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1276,7 +1276,7 @@
   <dimension ref="A1:S281"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="R1" sqref="R1:X60"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>